<commit_message>
new cards for gunslinger
</commit_message>
<xml_diff>
--- a/Card_Database.xlsx
+++ b/Card_Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Starter" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="419">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -303,16 +303,76 @@
     <t xml:space="preserve">Shoot</t>
   </si>
   <si>
-    <t xml:space="preserve">Use one ammo.</t>
+    <t xml:space="preserve">Use one ammo. Draw a card.</t>
   </si>
   <si>
     <t xml:space="preserve">Unload</t>
   </si>
   <si>
-    <t xml:space="preserve">Use all ammo.</t>
+    <t xml:space="preserve">Use all ammo. Deal 1 damage for each ammo consumed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burst Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use up to 3 ammo. Gain 1 energy for each ammo consumed.</t>
   </si>
   <si>
     <t xml:space="preserve">Ammo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piercing Round</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This target all enemies this turn. Deal 1 damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Bullet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enemy deals no damage this turn. Exhaust when consumed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hollow Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deal 4 damage if there is no ammo stored after this attack.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explosive Round</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The next attack against enemy this turn deals double damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incendiary Round</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This attack deals double damage. Exhaust when consumed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buckshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deal 2 damage for each ammo remaining when consumed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take Cover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain 2 block. Block does not deplete at the end of this turn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load any ammo found in your discard pile.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smoke Grenade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All allies gain 1 block from attacks this turn.</t>
   </si>
   <si>
     <t xml:space="preserve">Evicerate</t>
@@ -1589,10 +1649,10 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>40</v>
@@ -1600,10 +1660,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>15</v>
@@ -1611,10 +1671,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>10</v>
@@ -1622,10 +1682,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>5</v>
@@ -1633,10 +1693,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>2</v>
@@ -1644,10 +1704,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>2</v>
@@ -1655,10 +1715,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>2</v>
@@ -1666,10 +1726,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>2</v>
@@ -1677,10 +1737,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>2</v>
@@ -1704,8 +1764,8 @@
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1729,10 +1789,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
@@ -1740,10 +1800,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
@@ -1751,10 +1811,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
@@ -1762,10 +1822,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
@@ -1773,10 +1833,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>353</v>
+        <v>373</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>354</v>
+        <v>374</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
@@ -1784,10 +1844,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
@@ -1795,10 +1855,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>358</v>
+        <v>378</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
@@ -1806,10 +1866,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
@@ -1817,10 +1877,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>362</v>
+        <v>382</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
@@ -1828,10 +1888,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>363</v>
+        <v>383</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -1839,10 +1899,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>366</v>
+        <v>386</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
@@ -1850,10 +1910,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>367</v>
+        <v>387</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
@@ -1861,10 +1921,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>370</v>
+        <v>390</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
@@ -1872,10 +1932,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>371</v>
+        <v>391</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>372</v>
+        <v>392</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
@@ -1883,10 +1943,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
@@ -1894,10 +1954,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>376</v>
+        <v>396</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -1905,10 +1965,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -1916,10 +1976,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -1927,10 +1987,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>1</v>
@@ -1938,10 +1998,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>383</v>
+        <v>403</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>384</v>
+        <v>404</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>1</v>
@@ -1949,10 +2009,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>386</v>
+        <v>406</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>1</v>
@@ -1960,10 +2020,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>387</v>
+        <v>407</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>388</v>
+        <v>408</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
@@ -1971,10 +2031,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>389</v>
+        <v>409</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>1</v>
@@ -1982,10 +2042,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>392</v>
+        <v>412</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
@@ -1993,10 +2053,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>393</v>
+        <v>413</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>394</v>
+        <v>414</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>1</v>
@@ -2004,10 +2064,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>396</v>
+        <v>416</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>1</v>
@@ -2015,10 +2075,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>397</v>
+        <v>417</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>398</v>
+        <v>418</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>1</v>
@@ -2862,10 +2922,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2922,19 +2982,39 @@
         <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2942,18 +3022,209 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="2" t="n">
+        <v>4</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3009,7 +3280,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>31</v>
@@ -3024,12 +3295,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>40</v>
@@ -3044,12 +3315,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -3064,12 +3335,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>40</v>
@@ -3084,12 +3355,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>40</v>
@@ -3104,12 +3375,12 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>40</v>
@@ -3124,12 +3395,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>50</v>
@@ -3144,12 +3415,12 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>31</v>
@@ -3158,18 +3429,18 @@
         <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>31</v>
@@ -3178,18 +3449,18 @@
         <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>50</v>
@@ -3198,18 +3469,18 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>40</v>
@@ -3218,18 +3489,18 @@
         <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>50</v>
@@ -3238,18 +3509,18 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>40</v>
@@ -3258,18 +3529,18 @@
         <v>4</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>31</v>
@@ -3278,18 +3549,18 @@
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>31</v>
@@ -3298,18 +3569,18 @@
         <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>40</v>
@@ -3318,13 +3589,13 @@
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3380,7 +3651,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>31</v>
@@ -3395,12 +3666,12 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>31</v>
@@ -3415,12 +3686,12 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -3435,12 +3706,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -3455,12 +3726,12 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
@@ -3475,12 +3746,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>40</v>
@@ -3495,12 +3766,12 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>50</v>
@@ -3515,12 +3786,12 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>50</v>
@@ -3535,12 +3806,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>50</v>
@@ -3555,12 +3826,12 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>50</v>
@@ -3575,12 +3846,12 @@
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>31</v>
@@ -3595,12 +3866,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>31</v>
@@ -3620,7 +3891,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>31</v>
@@ -3635,12 +3906,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -3655,12 +3926,12 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>40</v>
@@ -3675,12 +3946,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>40</v>
@@ -3695,12 +3966,12 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>40</v>
@@ -3715,12 +3986,12 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>50</v>
@@ -3735,12 +4006,12 @@
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>31</v>
@@ -3749,18 +4020,18 @@
         <v>8</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E20" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>31</v>
@@ -3769,18 +4040,18 @@
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>31</v>
@@ -3789,18 +4060,18 @@
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>40</v>
@@ -3809,18 +4080,18 @@
         <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>40</v>
@@ -3829,18 +4100,18 @@
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>40</v>
@@ -3849,18 +4120,18 @@
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>40</v>
@@ -3869,18 +4140,18 @@
         <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>50</v>
@@ -3889,18 +4160,18 @@
         <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>50</v>
@@ -3909,13 +4180,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3951,13 +4222,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -3968,7 +4239,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>4</v>
@@ -3982,7 +4253,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -3996,7 +4267,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -4010,7 +4281,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -4066,281 +4337,281 @@
         <v>4</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -4368,7 +4639,7 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="8.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="40.15"/>
@@ -4389,39 +4660,39 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>1</v>
@@ -4430,36 +4701,36 @@
         <v>20</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
@@ -4468,7 +4739,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>2</v>
@@ -4483,21 +4754,21 @@
         <v>34</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
@@ -4506,36 +4777,36 @@
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>1</v>
@@ -4544,7 +4815,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>2</v>
@@ -4559,21 +4830,21 @@
         <v>34</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
@@ -4582,36 +4853,36 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
@@ -4620,36 +4891,36 @@
         <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
@@ -4658,36 +4929,36 @@
         <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
@@ -4696,36 +4967,36 @@
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
@@ -4734,36 +5005,36 @@
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -4772,36 +5043,36 @@
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
@@ -4810,36 +5081,36 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
@@ -4848,36 +5119,36 @@
         <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
@@ -4886,36 +5157,36 @@
         <v>50</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
@@ -4924,36 +5195,36 @@
         <v>30</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
@@ -4962,36 +5233,36 @@
         <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -5000,25 +5271,25 @@
         <v>80</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>6</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>82</v>
@@ -5026,10 +5297,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -5038,36 +5309,36 @@
         <v>100</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>6</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -5076,33 +5347,33 @@
         <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>6</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
     </row>
     <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -5118,7 +5389,7 @@
     </row>
     <row r="21" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>

</xml_diff>

<commit_message>
additional changes to class cards
</commit_message>
<xml_diff>
--- a/Card_Database.xlsx
+++ b/Card_Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Starter" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,7 @@
     <sheet name="Ironclad" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Gunslinger" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Trapper" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Sheet13" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Elementalist" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Mesmer" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Character" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Event" sheetId="9" state="visible" r:id="rId10"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="483">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -238,22 +238,25 @@
     <t xml:space="preserve">Gain 2 energy. Lose 1 HP.</t>
   </si>
   <si>
+    <t xml:space="preserve">Parry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whenever you play an Attack, gain 1 block.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrench</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double your block.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rage</t>
   </si>
   <si>
-    <t xml:space="preserve">Whenever you play an Attack, gain 1 block this turn.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entrench</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Double your block.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limit Break</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Double your strength.</t>
+    <t xml:space="preserve">Doubles the effect of strength.</t>
   </si>
   <si>
     <t xml:space="preserve">Offering</t>
@@ -262,10 +265,10 @@
     <t xml:space="preserve">Gain 2 energy. Draw 2 cards. Lose 2 HP.</t>
   </si>
   <si>
-    <t xml:space="preserve">Double Tap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This turn, your next Attack is played twice.</t>
+    <t xml:space="preserve">Flurry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your first attack each turn is played twice.</t>
   </si>
   <si>
     <t xml:space="preserve">Impervious</t>
@@ -397,7 +400,7 @@
     <t xml:space="preserve">All ammo now costs 0. When an ammo is consumed, exhaust it instead.</t>
   </si>
   <si>
-    <t xml:space="preserve">Evicerate</t>
+    <t xml:space="preserve">Decompose</t>
   </si>
   <si>
     <t xml:space="preserve">Deal damage equal to target’s poison.</t>
@@ -421,6 +424,12 @@
     <t xml:space="preserve">This turn, target deals X less attack damage, where X is the number of poison stacks on enemy.</t>
   </si>
   <si>
+    <t xml:space="preserve">Potency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whenever you apply poison, apply 1 additional stack.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Snake Venom</t>
   </si>
   <si>
@@ -508,25 +517,25 @@
     <t xml:space="preserve">Earth</t>
   </si>
   <si>
-    <t xml:space="preserve">Mantra of Fire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mantra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mantra of Air</t>
+    <t xml:space="preserve">Signet of Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signet of Air</t>
   </si>
   <si>
     <t xml:space="preserve">Draw 1 card.</t>
   </si>
   <si>
-    <t xml:space="preserve">Mantra of Water</t>
+    <t xml:space="preserve">Signet of Water</t>
   </si>
   <si>
     <t xml:space="preserve">Block does not expire this turn.</t>
   </si>
   <si>
-    <t xml:space="preserve">Mantra of Earth</t>
+    <t xml:space="preserve">Signet of Earth</t>
   </si>
   <si>
     <t xml:space="preserve">Gain 1 energy.</t>
@@ -559,7 +568,7 @@
     <t xml:space="preserve">Cinders</t>
   </si>
   <si>
-    <t xml:space="preserve">This turn, attacks deal 1 additional damage for each fire mantra.</t>
+    <t xml:space="preserve">Attacks deal 1 additional damage for each active fire mantra.</t>
   </si>
   <si>
     <t xml:space="preserve">Chain Lightning</t>
@@ -601,7 +610,7 @@
     <t xml:space="preserve">Obsidian Flesh</t>
   </si>
   <si>
-    <t xml:space="preserve">Incoming damage is reduced to 1 this turn. Exhaust.</t>
+    <t xml:space="preserve">Incoming damage is reduced by 1 (min. 1 damage).</t>
   </si>
   <si>
     <t xml:space="preserve">Unearth</t>
@@ -625,7 +634,7 @@
     <t xml:space="preserve">Conjure Frost</t>
   </si>
   <si>
-    <t xml:space="preserve">This turn, strike deals 1 additional damage for each water mantra.</t>
+    <t xml:space="preserve">This turn, Strikes deals 1 additional damage for each active water mantra.</t>
   </si>
   <si>
     <t xml:space="preserve">Ice Prison</t>
@@ -635,6 +644,27 @@
   </si>
   <si>
     <t xml:space="preserve">Frost Armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negates the next source of damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tidal Wave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target heal 1 HP. Exhaust.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maelstorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each time you are attacked, deal 1 damage for each active water mantra.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master of Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While attuned to three different elements, all skills cost 0.</t>
   </si>
   <si>
     <t xml:space="preserve">Shatter Illusions</t>
@@ -1815,39 +1845,39 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>1</v>
@@ -1856,36 +1886,36 @@
         <v>20</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
@@ -1894,7 +1924,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>2</v>
@@ -1909,21 +1939,21 @@
         <v>34</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
@@ -1932,36 +1962,36 @@
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>344</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>334</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>1</v>
@@ -1970,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>2</v>
@@ -1985,21 +2015,21 @@
         <v>34</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
@@ -2008,36 +2038,36 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
@@ -2046,36 +2076,36 @@
         <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
@@ -2084,36 +2114,36 @@
         <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
@@ -2122,36 +2152,36 @@
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
@@ -2160,36 +2190,36 @@
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -2198,36 +2228,36 @@
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
@@ -2236,36 +2266,36 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
@@ -2274,36 +2304,36 @@
         <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
@@ -2312,36 +2342,36 @@
         <v>50</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
@@ -2350,36 +2380,36 @@
         <v>30</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
@@ -2388,36 +2418,36 @@
         <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -2426,36 +2456,36 @@
         <v>80</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>6</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -2464,36 +2494,36 @@
         <v>100</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>6</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -2502,33 +2532,33 @@
         <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>6</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
     </row>
     <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -2544,7 +2574,7 @@
     </row>
     <row r="21" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
@@ -2601,10 +2631,10 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>40</v>
@@ -2612,10 +2642,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>15</v>
@@ -2623,10 +2653,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>10</v>
@@ -2634,10 +2664,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>5</v>
@@ -2645,10 +2675,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>2</v>
@@ -2656,10 +2686,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>2</v>
@@ -2667,10 +2697,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>2</v>
@@ -2678,10 +2708,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>2</v>
@@ -2689,10 +2719,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>2</v>
@@ -2741,10 +2771,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
@@ -2752,10 +2782,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
@@ -2763,10 +2793,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
@@ -2774,10 +2804,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
@@ -2785,10 +2815,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
@@ -2796,10 +2826,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
@@ -2807,10 +2837,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
@@ -2818,10 +2848,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
@@ -2829,10 +2859,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
@@ -2840,10 +2870,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -2851,10 +2881,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
@@ -2862,10 +2892,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
@@ -2873,10 +2903,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>443</v>
+        <v>453</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
@@ -2884,10 +2914,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
@@ -2895,10 +2925,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
@@ -2906,10 +2936,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -2917,10 +2947,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -2928,10 +2958,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -2939,10 +2969,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>1</v>
@@ -2950,10 +2980,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>1</v>
@@ -2961,10 +2991,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>460</v>
+        <v>470</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>1</v>
@@ -2972,10 +3002,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
@@ -2983,10 +3013,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>463</v>
+        <v>473</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>1</v>
@@ -2994,10 +3024,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>466</v>
+        <v>476</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
@@ -3005,10 +3035,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>467</v>
+        <v>477</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>468</v>
+        <v>478</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>1</v>
@@ -3016,10 +3046,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>1</v>
@@ -3027,10 +3057,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>471</v>
+        <v>481</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>1</v>
@@ -3283,10 +3313,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3669,18 +3699,18 @@
         <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>40</v>
@@ -3695,12 +3725,12 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>50</v>
@@ -3709,18 +3739,18 @@
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>50</v>
@@ -3735,12 +3765,12 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>50</v>
@@ -3749,113 +3779,117 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="E25" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="6" t="s">
+    </row>
+    <row r="26" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="6" t="n">
+      <c r="C26" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="E26" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="2" t="s">
+    </row>
+    <row r="28" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="C28" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="2" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>88</v>
+      <c r="C29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3911,7 +3945,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>31</v>
@@ -3926,12 +3960,12 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -3946,12 +3980,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>31</v>
@@ -3966,7 +4000,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3974,7 +4008,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>0</v>
@@ -3985,7 +4019,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>1</v>
@@ -3993,7 +4027,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>31</v>
@@ -4002,7 +4036,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>1</v>
@@ -4013,7 +4047,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>31</v>
@@ -4022,18 +4056,18 @@
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>40</v>
@@ -4042,18 +4076,18 @@
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>50</v>
@@ -4062,18 +4096,18 @@
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -4082,18 +4116,18 @@
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>40</v>
@@ -4102,18 +4136,18 @@
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>40</v>
@@ -4122,18 +4156,18 @@
         <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>40</v>
@@ -4142,18 +4176,18 @@
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>50</v>
@@ -4162,18 +4196,18 @@
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>40</v>
@@ -4188,12 +4222,12 @@
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>40</v>
@@ -4208,12 +4242,12 @@
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>31</v>
@@ -4228,12 +4262,12 @@
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>40</v>
@@ -4248,7 +4282,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4270,7 +4304,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4304,7 +4338,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>31</v>
@@ -4319,12 +4353,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>40</v>
@@ -4339,12 +4373,12 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -4359,12 +4393,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>40</v>
@@ -4379,12 +4413,32 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>40</v>
@@ -4393,18 +4447,18 @@
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>40</v>
@@ -4419,12 +4473,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>50</v>
@@ -4439,12 +4493,12 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>31</v>
@@ -4453,18 +4507,18 @@
         <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>31</v>
@@ -4473,18 +4527,18 @@
         <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>50</v>
@@ -4493,18 +4547,18 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>40</v>
@@ -4513,18 +4567,18 @@
         <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>50</v>
@@ -4533,18 +4587,18 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>40</v>
@@ -4553,18 +4607,18 @@
         <v>4</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>31</v>
@@ -4573,18 +4627,18 @@
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>31</v>
@@ -4593,18 +4647,18 @@
         <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>40</v>
@@ -4613,13 +4667,13 @@
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -4638,10 +4692,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4667,16 +4721,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -4687,7 +4741,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>31</v>
@@ -4695,8 +4749,8 @@
       <c r="C2" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>159</v>
+      <c r="D2" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>0</v>
@@ -4719,7 +4773,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>31</v>
@@ -4728,7 +4782,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E3" s="8" t="n">
         <v>0</v>
@@ -4746,12 +4800,12 @@
         <v>0</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -4760,7 +4814,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E4" s="8" t="n">
         <v>0</v>
@@ -4778,12 +4832,12 @@
         <v>0</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -4792,7 +4846,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>0</v>
@@ -4810,7 +4864,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4826,13 +4880,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="8" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>8</v>
@@ -4853,18 +4907,18 @@
         <v>1</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="8" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>8</v>
@@ -4885,12 +4939,12 @@
         <v>1</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>50</v>
@@ -4914,15 +4968,15 @@
         <v>0</v>
       </c>
       <c r="I9" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>40</v>
@@ -4949,12 +5003,12 @@
         <v>0</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>40</v>
@@ -4963,7 +5017,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="E11" s="8" t="n">
         <v>1</v>
@@ -4978,10 +5032,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4996,28 +5050,49 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="A13" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="8" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E14" s="8" t="n">
         <v>0</v>
@@ -5032,21 +5107,21 @@
         <v>0</v>
       </c>
       <c r="I14" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C15" s="8" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>11</v>
@@ -5055,7 +5130,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="8" t="n">
         <v>0</v>
@@ -5064,15 +5139,15 @@
         <v>0</v>
       </c>
       <c r="I15" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>40</v>
@@ -5099,107 +5174,128 @@
         <v>1</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="8" t="n">
+      <c r="C20" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="G18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="D20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C21" s="8" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E21" s="8" t="n">
         <v>0</v>
@@ -5211,24 +5307,24 @@
         <v>0</v>
       </c>
       <c r="H21" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>45</v>
+        <v>3</v>
+      </c>
+      <c r="I21" s="8" t="n">
+        <v>1</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C22" s="8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>11</v>
@@ -5243,24 +5339,24 @@
         <v>0</v>
       </c>
       <c r="H22" s="8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C23" s="8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>11</v>
@@ -5275,50 +5371,29 @@
         <v>0</v>
       </c>
       <c r="H23" s="8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I23" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>193</v>
-      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>40</v>
@@ -5336,70 +5411,91 @@
         <v>0</v>
       </c>
       <c r="G25" s="8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25" s="8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I25" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="A26" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>197</v>
+        <v>203</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>11</v>
@@ -5411,24 +5507,80 @@
         <v>0</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H28" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -5449,8 +5601,8 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5484,7 +5636,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>31</v>
@@ -5499,12 +5651,12 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>31</v>
@@ -5519,12 +5671,12 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -5539,12 +5691,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -5559,12 +5711,12 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
@@ -5579,12 +5731,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>40</v>
@@ -5599,12 +5751,12 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>50</v>
@@ -5619,12 +5771,12 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>50</v>
@@ -5639,12 +5791,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>50</v>
@@ -5659,12 +5811,12 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>50</v>
@@ -5679,12 +5831,12 @@
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>31</v>
@@ -5699,12 +5851,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>31</v>
@@ -5724,7 +5876,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>31</v>
@@ -5739,12 +5891,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -5759,12 +5911,12 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>40</v>
@@ -5779,12 +5931,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>40</v>
@@ -5799,12 +5951,12 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>40</v>
@@ -5819,12 +5971,12 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>50</v>
@@ -5839,12 +5991,12 @@
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>31</v>
@@ -5853,18 +6005,18 @@
         <v>8</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E20" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>31</v>
@@ -5873,18 +6025,18 @@
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>31</v>
@@ -5893,18 +6045,18 @@
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>40</v>
@@ -5913,18 +6065,18 @@
         <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>40</v>
@@ -5933,18 +6085,18 @@
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>40</v>
@@ -5953,18 +6105,18 @@
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>40</v>
@@ -5973,18 +6125,18 @@
         <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>50</v>
@@ -5993,18 +6145,18 @@
         <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>50</v>
@@ -6013,13 +6165,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>3</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -6055,13 +6207,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -6072,7 +6224,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>4</v>
@@ -6086,7 +6238,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -6100,7 +6252,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -6114,7 +6266,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -6170,281 +6322,281 @@
         <v>4</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to gameboard and character cards
</commit_message>
<xml_diff>
--- a/Card_Database.xlsx
+++ b/Card_Database.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="504">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -415,13 +415,55 @@
     <t xml:space="preserve">Poison Dagger</t>
   </si>
   <si>
-    <t xml:space="preserve">Apply 1 poison.</t>
+    <t xml:space="preserve">Deal 1 damage and apply 1 poison.</t>
   </si>
   <si>
     <t xml:space="preserve">Enfeeble</t>
   </si>
   <si>
-    <t xml:space="preserve">This turn, target deals X less attack damage, where X is the number of poison stacks on enemy.</t>
+    <t xml:space="preserve">Remove 1 poison from enemy. Gain 4 block.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain 3 block.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain 2 block. Draw a card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain 1 block. Draw a card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catalyst X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target gains 1 strength and loses 1 HP for each poison stack. Exhaust.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer all poison from one target to another. Exhaust.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toxic Cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All allies and enemies gain 2 stack of poison.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noxious Fumes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the start of your turn, all enemies gain 1 stack of poison.</t>
   </si>
   <si>
     <t xml:space="preserve">Potency</t>
@@ -433,7 +475,7 @@
     <t xml:space="preserve">Snake Venom</t>
   </si>
   <si>
-    <t xml:space="preserve">Every trap that triggers this turn applies 1 poison.</t>
+    <t xml:space="preserve">Every trap also applies 1 poison.</t>
   </si>
   <si>
     <t xml:space="preserve">Scavenge</t>
@@ -442,7 +484,7 @@
     <t xml:space="preserve">Move an exhausted Trap to your hand.</t>
   </si>
   <si>
-    <t xml:space="preserve">Preparedness</t>
+    <t xml:space="preserve">Craftsmanship</t>
   </si>
   <si>
     <t xml:space="preserve">This turn, all traps trigger twice.</t>
@@ -454,7 +496,7 @@
     <t xml:space="preserve">Trap</t>
   </si>
   <si>
-    <t xml:space="preserve">When attacked next, deal 4 damage to attacker.</t>
+    <t xml:space="preserve">When attacked next, deal 3 damage to attacker.</t>
   </si>
   <si>
     <t xml:space="preserve">Dust Trap</t>
@@ -472,7 +514,7 @@
     <t xml:space="preserve">Healing Spring</t>
   </si>
   <si>
-    <t xml:space="preserve">When attacked next, gain 2 HP.</t>
+    <t xml:space="preserve">When attacked next, defender gains 2 HP.</t>
   </si>
   <si>
     <t xml:space="preserve">Smoke Trap</t>
@@ -496,7 +538,7 @@
     <t xml:space="preserve">Tripwire</t>
   </si>
   <si>
-    <t xml:space="preserve">When attacked next, reduce damage by 2.</t>
+    <t xml:space="preserve">When attacked next, reduce damage by 1.</t>
   </si>
   <si>
     <t xml:space="preserve">Spike Trap</t>
@@ -652,7 +694,7 @@
     <t xml:space="preserve">Tidal Wave</t>
   </si>
   <si>
-    <t xml:space="preserve">Target heals 1 HP. Exhaust.</t>
+    <t xml:space="preserve">Remove all poison from target and heals 1 HP. Exhaust.</t>
   </si>
   <si>
     <t xml:space="preserve">Maelstorm</t>
@@ -1372,6 +1414,12 @@
     <t xml:space="preserve">At the start of each combat, put any Skill from your deck into your hand.</t>
   </si>
   <si>
+    <t xml:space="preserve">Bottled Tornado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the start of each combat, put any Power from your deck into your hand.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shuriken</t>
   </si>
   <si>
@@ -1459,7 +1507,7 @@
     <t xml:space="preserve">Maurader's Map</t>
   </si>
   <si>
-    <t xml:space="preserve">When you enter a new level, you can swap the contents of two rooms.</t>
+    <t xml:space="preserve">When you start a new stage, you can swap the contents of two rooms.</t>
   </si>
   <si>
     <t xml:space="preserve">Matryoshka</t>
@@ -1742,7 +1790,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1832,7 +1880,7 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1860,39 +1908,39 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>342</v>
+        <v>356</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>1</v>
@@ -1901,36 +1949,36 @@
         <v>20</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
@@ -1939,7 +1987,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>2</v>
@@ -1954,21 +2002,21 @@
         <v>34</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
@@ -1977,36 +2025,36 @@
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>354</v>
+        <v>368</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>356</v>
+        <v>370</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>356</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>1</v>
@@ -2015,7 +2063,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>2</v>
@@ -2030,21 +2078,21 @@
         <v>34</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>347</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
@@ -2053,36 +2101,36 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
@@ -2091,36 +2139,36 @@
         <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
@@ -2129,36 +2177,36 @@
         <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
@@ -2167,36 +2215,36 @@
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
@@ -2205,36 +2253,36 @@
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>379</v>
+        <v>393</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -2243,36 +2291,36 @@
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
@@ -2281,36 +2329,36 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>382</v>
+        <v>396</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>384</v>
+        <v>398</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>384</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
@@ -2319,36 +2367,36 @@
         <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
@@ -2357,36 +2405,36 @@
         <v>50</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
@@ -2395,36 +2443,36 @@
         <v>30</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
@@ -2433,36 +2481,36 @@
         <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>400</v>
+        <v>414</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -2471,25 +2519,25 @@
         <v>80</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>402</v>
+        <v>416</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>6</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>83</v>
@@ -2497,10 +2545,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>403</v>
+        <v>417</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -2509,36 +2557,36 @@
         <v>100</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>6</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>407</v>
+        <v>421</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -2547,33 +2595,33 @@
         <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>6</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
     </row>
     <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>412</v>
+        <v>426</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -2589,7 +2637,7 @@
     </row>
     <row r="21" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
@@ -2621,7 +2669,7 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2646,10 +2694,10 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>414</v>
+        <v>428</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>415</v>
+        <v>429</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>40</v>
@@ -2657,10 +2705,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>416</v>
+        <v>430</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>417</v>
+        <v>431</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>15</v>
@@ -2668,10 +2716,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>419</v>
+        <v>433</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>10</v>
@@ -2679,10 +2727,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>421</v>
+        <v>435</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>5</v>
@@ -2690,10 +2738,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>423</v>
+        <v>437</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>2</v>
@@ -2701,10 +2749,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>424</v>
+        <v>438</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>425</v>
+        <v>439</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>2</v>
@@ -2712,10 +2760,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>427</v>
+        <v>441</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>2</v>
@@ -2723,10 +2771,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>429</v>
+        <v>443</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>2</v>
@@ -2734,10 +2782,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>2</v>
@@ -2759,10 +2807,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2784,45 +2832,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>446</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>448</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C4" s="2" t="n">
+        <v>450</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>439</v>
+        <v>453</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
@@ -2830,10 +2878,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>441</v>
+        <v>455</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
@@ -2841,10 +2889,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>443</v>
+        <v>457</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
@@ -2852,10 +2900,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>445</v>
+        <v>459</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
@@ -2863,10 +2911,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>447</v>
+        <v>461</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
@@ -2874,10 +2922,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>449</v>
+        <v>463</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
@@ -2885,10 +2933,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>451</v>
+        <v>465</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -2896,10 +2944,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>453</v>
+        <v>467</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
@@ -2907,10 +2955,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>455</v>
+        <v>469</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
@@ -2918,10 +2966,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
@@ -2929,10 +2977,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>459</v>
+        <v>473</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
@@ -2940,10 +2988,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>461</v>
+        <v>475</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
@@ -2951,10 +2999,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>463</v>
+        <v>477</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -2962,10 +3010,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>465</v>
+        <v>479</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -2973,10 +3021,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>466</v>
+        <v>480</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -2984,10 +3032,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>468</v>
+        <v>482</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>1</v>
@@ -2995,10 +3043,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>470</v>
+        <v>484</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>1</v>
@@ -3006,10 +3054,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>472</v>
+        <v>486</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>1</v>
@@ -3017,10 +3065,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>474</v>
+        <v>488</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
@@ -3028,10 +3076,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>1</v>
@@ -3039,10 +3087,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
@@ -3050,10 +3098,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>480</v>
+        <v>494</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>1</v>
@@ -3061,10 +3109,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>1</v>
@@ -3072,10 +3120,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>1</v>
@@ -3083,12 +3131,23 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="C29" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C30" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3110,7 +3169,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -3140,7 +3199,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3339,10 +3398,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3465,7 +3524,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6" t="n">
         <v>2</v>
@@ -3916,6 +3975,12 @@
       </c>
       <c r="F29" s="2" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="2" t="n">
+        <f aca="false">SUM(C2:C29)</f>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3936,8 +4001,8 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4327,10 +4392,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4422,29 +4487,69 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>40</v>
@@ -4453,52 +4558,12 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4522,69 +4587,109 @@
         <v>137</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>40</v>
@@ -4593,18 +4698,18 @@
         <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>50</v>
@@ -4613,58 +4718,18 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>31</v>
@@ -4673,7 +4738,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>1</v>
@@ -4687,19 +4752,159 @@
         <v>155</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -4720,8 +4925,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4747,16 +4952,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -4767,7 +4972,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>31</v>
@@ -4776,7 +4981,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>0</v>
@@ -4799,7 +5004,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>31</v>
@@ -4808,7 +5013,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="E3" s="8" t="n">
         <v>0</v>
@@ -4826,12 +5031,12 @@
         <v>0</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -4840,7 +5045,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="E4" s="8" t="n">
         <v>0</v>
@@ -4858,12 +5063,12 @@
         <v>0</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -4872,7 +5077,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>0</v>
@@ -4890,7 +5095,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4906,7 +5111,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -4933,12 +5138,12 @@
         <v>1</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>31</v>
@@ -4965,12 +5170,12 @@
         <v>1</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>50</v>
@@ -4997,12 +5202,12 @@
         <v>2</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>40</v>
@@ -5029,12 +5234,12 @@
         <v>0</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>40</v>
@@ -5061,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5077,7 +5282,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>31</v>
@@ -5104,12 +5309,12 @@
         <v>1</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>31</v>
@@ -5136,12 +5341,12 @@
         <v>0</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>40</v>
@@ -5168,12 +5373,12 @@
         <v>1</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>40</v>
@@ -5200,12 +5405,12 @@
         <v>1</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>50</v>
@@ -5232,7 +5437,7 @@
         <v>3</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5248,7 +5453,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>31</v>
@@ -5275,12 +5480,12 @@
         <v>45</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>40</v>
@@ -5307,12 +5512,12 @@
         <v>1</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>50</v>
@@ -5339,12 +5544,12 @@
         <v>1</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>31</v>
@@ -5371,12 +5576,12 @@
         <v>0</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>40</v>
@@ -5403,7 +5608,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5419,7 +5624,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>40</v>
@@ -5446,12 +5651,12 @@
         <v>1</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>50</v>
@@ -5478,12 +5683,12 @@
         <v>1</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>40</v>
@@ -5510,12 +5715,12 @@
         <v>2</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>31</v>
@@ -5542,12 +5747,12 @@
         <v>0</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>31</v>
@@ -5574,12 +5779,12 @@
         <v>1</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>40</v>
@@ -5606,12 +5811,12 @@
         <v>1</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>40</v>
@@ -5638,7 +5843,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -5659,8 +5864,8 @@
   </sheetPr>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5694,7 +5899,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>31</v>
@@ -5709,12 +5914,12 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>31</v>
@@ -5729,12 +5934,12 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>31</v>
@@ -5749,12 +5954,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -5769,12 +5974,12 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
@@ -5789,12 +5994,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>40</v>
@@ -5809,12 +6014,12 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>50</v>
@@ -5829,12 +6034,12 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>50</v>
@@ -5849,12 +6054,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>50</v>
@@ -5869,12 +6074,12 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>50</v>
@@ -5889,12 +6094,12 @@
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>31</v>
@@ -5909,12 +6114,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>31</v>
@@ -5934,7 +6139,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>31</v>
@@ -5949,12 +6154,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -5969,12 +6174,12 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>40</v>
@@ -5989,12 +6194,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>40</v>
@@ -6009,12 +6214,12 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>40</v>
@@ -6029,12 +6234,12 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>50</v>
@@ -6049,12 +6254,12 @@
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>31</v>
@@ -6063,18 +6268,18 @@
         <v>8</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E20" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>31</v>
@@ -6083,18 +6288,18 @@
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>31</v>
@@ -6103,18 +6308,18 @@
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>40</v>
@@ -6123,18 +6328,18 @@
         <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>40</v>
@@ -6143,18 +6348,18 @@
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>40</v>
@@ -6163,18 +6368,18 @@
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>40</v>
@@ -6183,18 +6388,18 @@
         <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>50</v>
@@ -6203,18 +6408,18 @@
         <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>50</v>
@@ -6223,16 +6428,16 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -6253,7 +6458,7 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -6268,13 +6473,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -6285,7 +6490,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>4</v>
@@ -6299,7 +6504,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -6313,7 +6518,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -6327,7 +6532,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -6357,7 +6562,7 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -6383,281 +6588,281 @@
         <v>4</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>307</v>
+        <v>321</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>309</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>310</v>
+        <v>324</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>328</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
touching up character cards
</commit_message>
<xml_diff>
--- a/Card_Database.xlsx
+++ b/Card_Database.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="509">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -1375,7 +1375,7 @@
     <t xml:space="preserve">Dumbbell</t>
   </si>
   <si>
-    <t xml:space="preserve">Start combats with +1 strength.</t>
+    <t xml:space="preserve">Start combats with 1 strength.</t>
   </si>
   <si>
     <t xml:space="preserve">Backpack</t>
@@ -1441,13 +1441,13 @@
     <t xml:space="preserve">Letter Opener</t>
   </si>
   <si>
-    <t xml:space="preserve">Every time you play 3 Skills in a single turn, deal 1 damage to ALL enemies.</t>
+    <t xml:space="preserve">Every time you play 3 Skills in a single turn, deal 2 damage to any target.</t>
   </si>
   <si>
     <t xml:space="preserve">Smiling Mask</t>
   </si>
   <si>
-    <t xml:space="preserve">The merchant's card removal cost is only 5 gold now.</t>
+    <t xml:space="preserve">All shop prices are reduced by 2.</t>
   </si>
   <si>
     <t xml:space="preserve">Charon's Ashes</t>
@@ -1459,13 +1459,10 @@
     <t xml:space="preserve">Ginger</t>
   </si>
   <si>
-    <t xml:space="preserve">You can no longer become weak.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ice Cream</t>
   </si>
   <si>
-    <t xml:space="preserve">Energy is now conserved between turns.</t>
+    <t xml:space="preserve">For any combat you enter alone, double rewards.</t>
   </si>
   <si>
     <t xml:space="preserve">Spinning Top</t>
@@ -1543,7 +1540,25 @@
     <t xml:space="preserve">Elemental Tome</t>
   </si>
   <si>
-    <t xml:space="preserve">Before each combat, you may put a signet from your deck in play.</t>
+    <t xml:space="preserve">Before each combat, you may put one sigil from your deck in play.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broken Glasses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each turn, play the top card of your deck for free. Draw one less card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark Matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All damage to allies is multiplied by two and redirected to you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select from 4 cards instead of 3 when you acquire Experience.</t>
   </si>
 </sst>
 </file>
@@ -2669,7 +2684,7 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2807,10 +2822,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2990,19 +3005,16 @@
       <c r="A16" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>475</v>
-      </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>477</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -3010,10 +3022,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>479</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -3021,10 +3033,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -3032,10 +3044,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>1</v>
@@ -3043,10 +3055,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>485</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>1</v>
@@ -3054,10 +3066,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>486</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>487</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>1</v>
@@ -3065,10 +3077,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>489</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
@@ -3076,10 +3088,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>491</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>1</v>
@@ -3087,10 +3099,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>493</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
@@ -3098,10 +3110,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>494</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>495</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>1</v>
@@ -3109,10 +3121,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>497</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>1</v>
@@ -3120,10 +3132,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>499</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>1</v>
@@ -3131,10 +3143,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>1</v>
@@ -3142,12 +3154,45 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="B31" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C33" s="2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to cards and board
</commit_message>
<xml_diff>
--- a/Card_Database.xlsx
+++ b/Card_Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Starter" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,6 @@
     <sheet name="Monster" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Treasure" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Relic" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Ironclad_Classic" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="568">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -449,10 +448,10 @@
     <t xml:space="preserve">Gain 1 block. Draw a card.</t>
   </si>
   <si>
-    <t xml:space="preserve">Catalyst X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target gains 1 strength and loses 1 HP for each poison stack. Exhaust.</t>
+    <t xml:space="preserve">Catalyst Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target gains 1 strength and loses 1 HP for each poison stack on them. Exhaust.</t>
   </si>
   <si>
     <t xml:space="preserve">Transfect</t>
@@ -938,10 +937,10 @@
     <t xml:space="preserve">The doors lock behind you. An alter with three pedestals covered in blood sits in the center of the room.</t>
   </si>
   <si>
-    <t xml:space="preserve">Lose 3 HP. Gain 1 treasure. Stay.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lose 3 HP. Gain 1 max HP. Stay.</t>
+    <t xml:space="preserve">Lose 3 HP. You gain 1 treasure. Stay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lose 3 HP. You gain 1 max HP. Stay.</t>
   </si>
   <si>
     <t xml:space="preserve">Lose 3 HP. Leave.</t>
@@ -977,7 +976,7 @@
     <t xml:space="preserve">The Rogue</t>
   </si>
   <si>
-    <t xml:space="preserve">Lose 7 gold. Remove a card from your deck.</t>
+    <t xml:space="preserve">Lose 7 gold. Remove a card from one deck.</t>
   </si>
   <si>
     <t xml:space="preserve">Move on.</t>
@@ -986,7 +985,7 @@
     <t xml:space="preserve">The Scavenger</t>
   </si>
   <si>
-    <t xml:space="preserve">Add two random cards to your deck.</t>
+    <t xml:space="preserve">Add two random cards to each deck.</t>
   </si>
   <si>
     <t xml:space="preserve">The Cleric</t>
@@ -1079,7 +1078,7 @@
     <t xml:space="preserve">Dark Corridor</t>
   </si>
   <si>
-    <t xml:space="preserve">You find a winding passage. A blue flame torch illuminates the entrance, as the only guiding light.</t>
+    <t xml:space="preserve">You find yourself in a winding passage. A blue flame torch illuminates the entrance, as the only guiding light.</t>
   </si>
   <si>
     <t xml:space="preserve">Find your own way. Teleport to the boss room for the level.</t>
@@ -1088,7 +1087,7 @@
     <t xml:space="preserve">Use the torch. Add a curse to your deck.</t>
   </si>
   <si>
-    <t xml:space="preserve">Library</t>
+    <t xml:space="preserve">Mahogany Library</t>
   </si>
   <si>
     <t xml:space="preserve">A massive library fill the room, with a padded chair in the center.</t>
@@ -1100,6 +1099,36 @@
     <t xml:space="preserve">Rest. Heal 5 HP.</t>
   </si>
   <si>
+    <t xml:space="preserve">Lullaby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listen. Replace each strike in your deck with a random card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allegro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listen. Replace each defend in your deck with a random card.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ominous Forge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forge. Gain 1 relic and add a curse to your deck.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove a card from your deck.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divine Fountain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove all curses from your deck.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Merchant</t>
   </si>
   <si>
@@ -1124,16 +1153,16 @@
     <t xml:space="preserve">Trainer</t>
   </si>
   <si>
-    <t xml:space="preserve">Draw five Character cards from each present player’s deck.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 gold: Add a common card to respective deck.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 gold: Add uncommon card to respective deck.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 gold: Add rare card to respective deck.</t>
+    <t xml:space="preserve">Draw five Character cards from each player’s deck.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 gold: Add a common card to your deck.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 gold: Add uncommon card to your deck.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 gold: Add rare card to your deck.</t>
   </si>
   <si>
     <t xml:space="preserve">Healer</t>
@@ -1517,7 +1546,7 @@
     <t xml:space="preserve">Smiling Mask</t>
   </si>
   <si>
-    <t xml:space="preserve">All shop prices are reduced by 2.</t>
+    <t xml:space="preserve">All shop prices are reduced by 2 (minimum 1 gold).</t>
   </si>
   <si>
     <t xml:space="preserve">Charon's Ashes</t>
@@ -1631,6 +1660,9 @@
     <t xml:space="preserve">Select from 4 cards instead of 3 when you acquire Experience.</t>
   </si>
   <si>
+    <t xml:space="preserve">Hammock</t>
+  </si>
+  <si>
     <t xml:space="preserve">Whenever you enter a camp, gain 2 max HP.</t>
   </si>
   <si>
@@ -1640,7 +1672,7 @@
     <t xml:space="preserve">Whenever an enemy dies, gain 1 energy and draw a card.</t>
   </si>
   <si>
-    <t xml:space="preserve">Whenever you play a Power, play a random card from your hand for free.</t>
+    <t xml:space="preserve">Whenever you play a Power, the next card you play costs 0 energy.</t>
   </si>
   <si>
     <t xml:space="preserve">When selecting a card to add to your deck, you can gain 1 max HP instead.</t>
@@ -1698,6 +1730,9 @@
   </si>
   <si>
     <t xml:space="preserve">You can now view the cards in your draw pile.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical X</t>
   </si>
   <si>
     <t xml:space="preserve">Effect of cards that cost X are increased by 2.</t>
@@ -1710,7 +1745,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1751,6 +1786,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -1807,7 +1847,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1852,15 +1892,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1947,7 +1991,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -2037,8 +2081,8 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2083,16 +2127,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,76 +2144,76 @@
         <v>304</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -2190,7 +2234,7 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -2218,39 +2262,39 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>377</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>378</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>380</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>382</v>
+        <v>386</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>1</v>
@@ -2259,36 +2303,36 @@
         <v>20</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>387</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>387</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>387</v>
+      <c r="G2" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
@@ -2297,36 +2341,36 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="13" t="s">
-        <v>389</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>389</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>389</v>
+      <c r="J3" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
@@ -2335,36 +2379,36 @@
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>392</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>392</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>392</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>392</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>393</v>
+      <c r="G4" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>394</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>384</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>1</v>
@@ -2373,36 +2417,36 @@
         <v>6</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>397</v>
+      <c r="J5" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
@@ -2411,36 +2455,36 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>387</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>387</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>400</v>
+      <c r="G6" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
@@ -2449,36 +2493,36 @@
         <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>404</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>404</v>
+      <c r="G7" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
@@ -2487,36 +2531,36 @@
         <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>407</v>
+      <c r="G8" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
@@ -2525,36 +2569,36 @@
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>410</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>410</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>410</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>410</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>410</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>411</v>
+      <c r="G9" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
@@ -2563,36 +2607,36 @@
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>415</v>
+      <c r="G10" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -2601,36 +2645,36 @@
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>396</v>
+      <c r="G11" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
@@ -2639,36 +2683,36 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>421</v>
+      <c r="G12" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>431</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
@@ -2677,36 +2721,36 @@
         <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>425</v>
+      <c r="G13" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
@@ -2715,36 +2759,36 @@
         <v>50</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>429</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>429</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>430</v>
+      <c r="G14" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>439</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>439</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
@@ -2753,36 +2797,36 @@
         <v>30</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>433</v>
+      <c r="G15" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
@@ -2791,36 +2835,36 @@
         <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>404</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>404</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>404</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>404</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>436</v>
+      <c r="G16" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -2829,36 +2873,36 @@
         <v>80</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="L17" s="13" t="s">
+      <c r="G17" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="L17" s="14" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -2867,36 +2911,36 @@
         <v>100</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>442</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>442</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>443</v>
+      <c r="G18" s="14" t="s">
+        <v>451</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>451</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>451</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>452</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>452</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -2905,61 +2949,61 @@
         <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="G19" s="13" t="s">
-        <v>446</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>448</v>
+      <c r="G19" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2979,7 +3023,7 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -3004,10 +3048,10 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>40</v>
@@ -3015,10 +3059,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>15</v>
@@ -3029,10 +3073,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>10</v>
@@ -3043,10 +3087,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>5</v>
@@ -3057,10 +3101,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>460</v>
+        <v>470</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>2</v>
@@ -3068,10 +3112,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>2</v>
@@ -3079,10 +3123,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>463</v>
+        <v>473</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>2</v>
@@ -3090,10 +3134,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>466</v>
+        <v>476</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>2</v>
@@ -3101,10 +3145,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>467</v>
+        <v>477</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>468</v>
+        <v>478</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>2</v>
@@ -3128,8 +3172,8 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3153,10 +3197,10 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>1</v>
@@ -3164,10 +3208,10 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>471</v>
+        <v>481</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>1</v>
@@ -3175,10 +3219,10 @@
     </row>
     <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>1</v>
@@ -3186,10 +3230,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
@@ -3197,10 +3241,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>478</v>
+        <v>488</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
@@ -3208,10 +3252,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>479</v>
+        <v>489</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>480</v>
+        <v>490</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
@@ -3219,10 +3263,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>481</v>
+        <v>491</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>482</v>
+        <v>492</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
@@ -3230,10 +3274,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>483</v>
+        <v>493</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>484</v>
+        <v>494</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
@@ -3241,10 +3285,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>485</v>
+        <v>495</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>486</v>
+        <v>496</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
@@ -3252,10 +3296,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>487</v>
+        <v>497</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -3263,10 +3307,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>489</v>
+        <v>499</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>1</v>
@@ -3274,10 +3318,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>491</v>
+        <v>501</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>492</v>
+        <v>502</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
@@ -3285,10 +3329,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>493</v>
+        <v>503</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>494</v>
+        <v>504</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
@@ -3296,10 +3340,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>495</v>
+        <v>505</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
@@ -3307,7 +3351,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
@@ -3315,10 +3359,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>498</v>
+        <v>508</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
@@ -3326,10 +3370,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
@@ -3337,10 +3381,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>503</v>
+        <v>513</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1</v>
@@ -3348,10 +3392,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>505</v>
+        <v>515</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>1</v>
@@ -3359,10 +3403,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>506</v>
+        <v>516</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>507</v>
+        <v>517</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>1</v>
@@ -3370,10 +3414,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>508</v>
+        <v>518</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>509</v>
+        <v>519</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>1</v>
@@ -3381,10 +3425,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>511</v>
+        <v>521</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
@@ -3392,10 +3436,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>512</v>
+        <v>522</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>513</v>
+        <v>523</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>1</v>
@@ -3403,10 +3447,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>514</v>
+        <v>524</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>515</v>
+        <v>525</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
@@ -3414,10 +3458,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>516</v>
+        <v>526</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>517</v>
+        <v>527</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>1</v>
@@ -3425,10 +3469,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>1</v>
@@ -3436,10 +3480,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>521</v>
+        <v>531</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>1</v>
@@ -3447,10 +3491,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>522</v>
+        <v>532</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>523</v>
+        <v>533</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>1</v>
@@ -3458,10 +3502,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>524</v>
+        <v>534</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>525</v>
+        <v>535</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>1</v>
@@ -3469,10 +3513,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>526</v>
+        <v>536</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>527</v>
+        <v>537</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>1</v>
@@ -3480,10 +3524,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>528</v>
+        <v>538</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>529</v>
+        <v>539</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>1</v>
@@ -3491,18 +3535,21 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>531</v>
+        <v>541</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>542</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>1</v>
@@ -3510,10 +3557,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>533</v>
+        <v>544</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>534</v>
+        <v>545</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>1</v>
@@ -3521,7 +3568,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>535</v>
+        <v>546</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>1</v>
@@ -3529,7 +3576,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="s">
-        <v>536</v>
+        <v>547</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>1</v>
@@ -3537,10 +3584,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>537</v>
+        <v>548</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>538</v>
+        <v>549</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>1</v>
@@ -3548,10 +3595,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>539</v>
+        <v>550</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>540</v>
+        <v>551</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>1</v>
@@ -3559,10 +3606,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>541</v>
+        <v>552</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>542</v>
+        <v>553</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>1</v>
@@ -3570,10 +3617,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>543</v>
+        <v>554</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>544</v>
+        <v>555</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>1</v>
@@ -3581,10 +3628,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>545</v>
+        <v>556</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>1</v>
@@ -3592,10 +3639,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>547</v>
+        <v>558</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>548</v>
+        <v>559</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>1</v>
@@ -3603,10 +3650,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>1</v>
@@ -3614,10 +3661,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>551</v>
+        <v>562</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>552</v>
+        <v>563</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>1</v>
@@ -3625,48 +3672,27 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>553</v>
+        <v>564</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>554</v>
+        <v>565</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>566</v>
+      </c>
       <c r="B47" s="2" t="s">
-        <v>555</v>
+        <v>567</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="65.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
-  </cols>
-  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3684,7 +3710,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3885,7 +3911,7 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -4480,7 +4506,7 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -4873,8 +4899,8 @@
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5424,7 +5450,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -6363,7 +6389,7 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -6991,7 +7017,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -7098,10 +7124,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7403,6 +7429,86 @@
         <v>354</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>315</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>